<commit_message>
Fan Tong, June 26, 2018 test commit
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mengyao @ Carnegie\research\models\SEM-1-master 180626\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2FF1AB47-6D3B-4526-B8DC-8E650CC0DF20}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ACF5BD-A862-4DC2-8E6C-A70FBD5035BD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15500" windowHeight="7940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7373" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Note that costs of technologies with associated capacity files (e.g., wind solar) are assumed to be of the form where fixed costs the cost of hour of acheiveing the potential generation in the associated capacity file (i.e., there is no further normalization within the code).</t>
   </si>
   <si>
-    <t>All power-related (i.e., generation) costs  are in terms of $/kWh dipatched</t>
-  </si>
-  <si>
     <t>Variable cost of energy storage (dispatch_cost_storage) is in units of $/hr per kWh stored.</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>GLOBAL_NAME</t>
   </si>
   <si>
-    <t>test5</t>
-  </si>
-  <si>
     <t>GLOBAL_NAME will be the name of the folder containing key output, name of pickle file, etc</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>DATA_PATH</t>
   </si>
   <si>
-    <t>Input_Data/Clack_EIA</t>
-  </si>
-  <si>
     <t>DATA_PATH is where the input data will reside. It is prepended to the wind, solar, and demand file specifications listed in the cases. (no trailing slash)</t>
   </si>
   <si>
@@ -136,9 +127,6 @@
     <t>DEMAND_FILE</t>
   </si>
   <si>
-    <t>demand_series_EIA_normalized_to_1_mean_synthetic_Clack.csv</t>
-  </si>
-  <si>
     <t>START_YEAR</t>
   </si>
   <si>
@@ -166,15 +154,9 @@
     <t>SOLAR_CAPACITY_FILE</t>
   </si>
   <si>
-    <t>solar_series_Clack_normalized_to_1_mean.csv</t>
-  </si>
-  <si>
     <t>CAPACITY_COST_SOLAR</t>
   </si>
   <si>
-    <t>$/kW</t>
-  </si>
-  <si>
     <t>DISPATCH_COST_SOLAR</t>
   </si>
   <si>
@@ -184,9 +166,6 @@
     <t>WIND_CAPACITY_FILE</t>
   </si>
   <si>
-    <t>wind_series_Clack_normalized_to_1_mean.csv</t>
-  </si>
-  <si>
     <t>CAPACITY_COST_WIND</t>
   </si>
   <si>
@@ -269,12 +248,84 @@
   </si>
   <si>
     <t>Note: values provided below will override values given above.</t>
+  </si>
+  <si>
+    <t>Input_Data/Shaner-et-al_E&amp;ES2018</t>
+  </si>
+  <si>
+    <t>solar_series_Shaner_normalized_to_0.2_mean.csv</t>
+  </si>
+  <si>
+    <t>wind_series_Shaner_normalized_to_0.38_mean.csv</t>
+  </si>
+  <si>
+    <t>demand_series_Shaner_normalized_to_1_mean.csv</t>
+  </si>
+  <si>
+    <t>CAPACITY_COST_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>DISPATCH_COST_TO_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>DISPATCH_COST_FROM_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>PGP_STORAGE_CHARGING_EFFICIENCY</t>
+  </si>
+  <si>
+    <t>CAPACITY_COST_PGP_FUEL_CELL</t>
+  </si>
+  <si>
+    <t>1e-6 adds on about 1 cent per kWh if used one cycle per year</t>
+  </si>
+  <si>
+    <t>This will add 1 cent per h per kW capacity</t>
+  </si>
+  <si>
+    <t>0.01 means 1 cent per hour per kW capacity</t>
+  </si>
+  <si>
+    <t>($/h)/kW</t>
+  </si>
+  <si>
+    <t>battery01</t>
+  </si>
+  <si>
+    <t>battery003</t>
+  </si>
+  <si>
+    <t>battery1</t>
+  </si>
+  <si>
+    <t>battery03</t>
+  </si>
+  <si>
+    <t>0.012 is default value for NGCC, 0.027 is default value for NGCC + CCS</t>
+  </si>
+  <si>
+    <t>0.021 is default value</t>
+  </si>
+  <si>
+    <t>0.020 is default value</t>
+  </si>
+  <si>
+    <t>All power-related (i.e., generation) costs  are in terms of $/kWh dispatched</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>0.062 is default value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -783,30 +834,30 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1162,712 +1213,778 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" style="8"/>
-    <col min="3" max="16384" width="16.6328125" style="1"/>
+    <col min="1" max="1" width="36.06640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.73046875" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.53125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-    </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="8"/>
-    </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="10"/>
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="8"/>
-    </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="9" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="10" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="B40" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+      <c r="C40" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="10" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="5"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="B42" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="10" t="b">
+      <c r="B43" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="5"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="10" t="b">
+      <c r="B45" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" s="5"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="12">
         <v>1</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="12">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="12">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="12">
+        <v>12</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="12">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="12">
+        <v>24</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61" s="5"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="14">
+        <v>1.9528741509529837E-2</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="13">
+        <f>0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="5"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="11">
-        <v>1000000000</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="11">
-        <v>1000000000</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" s="10">
-        <v>2006</v>
-      </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B54" s="10">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="10">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="10">
-        <v>1</v>
-      </c>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" s="10">
-        <v>2006</v>
-      </c>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58" s="10">
-        <v>12</v>
-      </c>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B59" s="10">
-        <v>31</v>
-      </c>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="10">
-        <v>24</v>
-      </c>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="5"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62" s="10" t="s">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
+      <c r="B67" s="14">
+        <v>2.0648572594225215E-2</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B68" s="13">
+        <v>2E-8</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="5"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" s="14">
+        <v>1.1841887362491711E-2</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="14">
+        <v>2.2590009128958689E-2</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B63" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" s="10">
-        <v>1E-4</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="5"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="10" t="s">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="5"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
+      <c r="B73" s="14">
+        <v>6.2433901191501419E-2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B67" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C67" s="2" t="s">
+      <c r="B74" s="14">
+        <v>2.5158160216169324E-2</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="5"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="5" t="s">
+      <c r="B76" s="14">
+        <v>8.1211742157245251E-3</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B68" s="10">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="C68" s="2" t="s">
+      <c r="B77" s="12">
+        <v>0</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="5"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="5" t="s">
+      <c r="B78" s="12">
+        <v>0</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B70" s="10">
-        <v>3</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
+      <c r="B79" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B71" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="5"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
+      <c r="B80" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B73" s="10">
-        <v>5.5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B74" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="5"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B76" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77" s="10">
-        <v>0</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" s="10">
-        <v>0</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B79" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" s="10">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="D80" s="2"/>
       <c r="E80" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="12">
+        <v>4</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82" s="5"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="12">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="12">
+        <v>0</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" s="12">
+        <v>0</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88" s="5"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B89" s="12">
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C91" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A95" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B95" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A96" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B96" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B97" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A98" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+      <c r="B100" s="11"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A104" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B81" s="10">
-        <v>4</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A82" s="5"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A83" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B83" s="10">
-        <v>1000</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C85" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C86" s="4"/>
-    </row>
-    <row r="87" spans="1:14" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K87" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L87" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M87" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="N87" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="6">
-        <v>1</v>
-      </c>
-      <c r="B89" s="11">
-        <v>2.3E-2</v>
-      </c>
-      <c r="C89" s="6">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D89" s="6">
-        <v>2.3E-2</v>
-      </c>
-      <c r="E89" s="6">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="F89" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="G89" s="6">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H89" s="6">
-        <v>5.5E-2</v>
-      </c>
-      <c r="I89" s="6">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="J89" s="6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="K89" s="6">
-        <v>0</v>
-      </c>
-      <c r="L89" s="6">
-        <v>0</v>
-      </c>
-      <c r="M89" s="6">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="N89" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B91" s="9"/>
-    </row>
-    <row r="95" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some digits to default values in case_input.xlsx
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mengyao @ Carnegie\research\models\SEM-1-master 180626\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206241D6-51A2-4E3D-B1B0-8A0B5A0B74B5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9799C2A4-F26B-4DC2-A727-3344E6CC5744}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7373" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>This will add 1 cent per h per kW capacity</t>
   </si>
   <si>
-    <t>0.01 means 1 cent per hour per kW capacity</t>
-  </si>
-  <si>
     <t>($/h)/kW</t>
   </si>
   <si>
@@ -301,22 +298,25 @@
     <t>battery03</t>
   </si>
   <si>
-    <t>0.012 is default value for NGCC, 0.027 is default value for NGCC + CCS</t>
-  </si>
-  <si>
-    <t>0.021 is default value</t>
-  </si>
-  <si>
-    <t>0.020 is default value</t>
-  </si>
-  <si>
     <t>All power-related (i.e., generation) costs  are in terms of $/kWh dispatched</t>
   </si>
   <si>
     <t>example</t>
   </si>
   <si>
-    <t>0.062 is default value</t>
+    <t>0.01953 is default value</t>
+  </si>
+  <si>
+    <t>0.02065 is default value</t>
+  </si>
+  <si>
+    <t>0.01184 is default value for NGCC, 0.027 is default value for NGCC + CCS</t>
+  </si>
+  <si>
+    <t>0.06243 is default value</t>
+  </si>
+  <si>
+    <t>0.00812 is the default value; 0.01 means 1 cent per hour per kW capacity</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -856,7 +856,7 @@
     <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1216,183 +1216,183 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.06640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.73046875" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.53125" style="1"/>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -1400,18 +1400,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -1422,12 +1422,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -1449,12 +1449,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="12"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>30</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>71</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>72</v>
       </c>
@@ -1487,10 +1487,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>32</v>
       </c>
@@ -1499,10 +1499,10 @@
       </c>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>34</v>
       </c>
@@ -1511,13 +1511,13 @@
       </c>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="12"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>36</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>37</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>38</v>
       </c>
@@ -1557,7 +1557,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>39</v>
       </c>
@@ -1567,7 +1567,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>40</v>
       </c>
@@ -1577,7 +1577,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>41</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>42</v>
       </c>
@@ -1597,13 +1597,13 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="12"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>43</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>44</v>
       </c>
@@ -1621,13 +1621,13 @@
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>45</v>
       </c>
@@ -1640,13 +1640,13 @@
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="12"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>47</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>48</v>
       </c>
@@ -1664,13 +1664,13 @@
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>50</v>
       </c>
@@ -1682,13 +1682,13 @@
       </c>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="12"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>52</v>
       </c>
@@ -1696,13 +1696,13 @@
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -1714,13 +1714,13 @@
       </c>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="12"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>54</v>
       </c>
@@ -1728,13 +1728,13 @@
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>55</v>
       </c>
@@ -1746,13 +1746,13 @@
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="12"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>56</v>
       </c>
@@ -1760,13 +1760,13 @@
         <v>8.1211742157245251E-3</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>57</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>58</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>59</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>60</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>63</v>
       </c>
@@ -1830,13 +1830,13 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="12"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>80</v>
       </c>
@@ -1844,13 +1844,13 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>84</v>
       </c>
@@ -1858,13 +1858,13 @@
         <v>0.01</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>81</v>
       </c>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>82</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>83</v>
       </c>
@@ -1898,13 +1898,13 @@
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="12"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>65</v>
       </c>
@@ -1916,15 +1916,15 @@
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C91" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>66</v>
       </c>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>68</v>
       </c>
@@ -1941,48 +1941,48 @@
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B95" s="8">
         <v>0.01</v>
       </c>
     </row>
-    <row r="96" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" s="8">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B97" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B98" s="8">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B100" s="11"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
preparing Fans quicklook functions
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9799C2A4-F26B-4DC2-A727-3344E6CC5744}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2AC576-86CA-49BB-8A07-01DF39215CE7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21590" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t>0.00812 is the default value; 0.01 means 1 cent per hour per kW capacity</t>
+  </si>
+  <si>
+    <t>QUICKLOOK</t>
+  </si>
+  <si>
+    <t>QUICKLOOK is true if you want to use the newer postprocessing system.</t>
   </si>
 </sst>
 </file>
@@ -1214,185 +1220,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -1422,12 +1428,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -1449,97 +1455,98 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="5"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B46" s="13">
-        <v>1000000000</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="B47" s="13">
         <v>1000000000</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="12"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B53" s="12">
-        <v>2006</v>
-      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="5"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" s="12">
-        <v>1</v>
+        <v>2006</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B55" s="12">
         <v>1</v>
@@ -1547,9 +1554,9 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B56" s="12">
         <v>1</v>
@@ -1557,230 +1564,228 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="12">
-        <v>2006</v>
+        <v>1</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" s="12">
-        <v>12</v>
+        <v>2006</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" s="12">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B60" s="12">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="12"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="12">
+        <v>24</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>77</v>
-      </c>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="5"/>
+      <c r="B62" s="12"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="14">
+      <c r="B64" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B64" s="13">
+      <c r="B65" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>78</v>
-      </c>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="5"/>
+      <c r="B66" s="12"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B67" s="14">
+      <c r="B68" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="13">
+      <c r="B69" s="13">
         <v>2E-8</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="5"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="14">
+      <c r="B71" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B72" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="5"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B73" s="14">
+      <c r="B74" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B74" s="14">
+      <c r="B75" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="5"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="14">
+      <c r="B77" s="14">
         <v>8.1211742157245251E-3</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B77" s="12">
-        <v>0</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="B78" s="12">
         <v>0</v>
@@ -1790,95 +1795,95 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B79" s="12">
+        <v>0</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B79" s="12">
+      <c r="B80" s="12">
         <v>0.9</v>
       </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B80" s="12">
+      <c r="B81" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="1">
+      <c r="D81" s="2"/>
+      <c r="E81" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B81" s="12">
+      <c r="B82" s="12">
         <v>4</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="5"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="12">
+      <c r="B84" s="12">
         <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B84" s="12">
-        <v>0.01</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D84" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B85" s="12">
-        <v>0</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="B86" s="12">
         <v>0</v>
@@ -1888,102 +1893,114 @@
       </c>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="12">
+        <v>0</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B87" s="12">
+      <c r="B88" s="12">
         <v>0.3</v>
       </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="12"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="5"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B89" s="12">
+      <c r="B90" s="12">
         <v>10</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="2" t="s">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C92" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="93" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B93" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C92" s="4"/>
-    </row>
-    <row r="93" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B94" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B95" s="8">
+      <c r="B96" s="8">
         <v>0.01</v>
       </c>
     </row>
-    <row r="96" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B96" s="8">
+      <c r="B97" s="8">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B97" s="8">
+      <c r="B98" s="8">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+    <row r="99" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B98" s="8">
+      <c r="B99" s="8">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+    <row r="101" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B100" s="11"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="B101" s="11"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor fix of in Save_Basic_Results. Working on Quick_look
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2AC576-86CA-49BB-8A07-01DF39215CE7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEF92F1-DE24-46FB-AD1F-7E5B10D858E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21590" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>QUICKLOOK is true if you want to use the newer postprocessing system.</t>
+  </si>
+  <si>
+    <t>NORMALIZE_DEMAND_TO_ONE</t>
+  </si>
+  <si>
+    <t>Normalize demand to 1.</t>
   </si>
 </sst>
 </file>
@@ -1220,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1473,90 +1479,91 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>76</v>
+        <v>101</v>
+      </c>
+      <c r="B46" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="13">
-        <v>1000000000</v>
+        <v>30</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" s="13">
         <v>1000000000</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B51" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C51" s="2"/>
+      <c r="C51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="5"/>
-      <c r="B53" s="12"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="12">
-        <v>2006</v>
-      </c>
+      <c r="A54" s="5"/>
+      <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" s="12">
-        <v>1</v>
+        <v>2006</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B56" s="12">
         <v>1</v>
@@ -1566,7 +1573,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="12">
         <v>1</v>
@@ -1576,228 +1583,226 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="12">
-        <v>2006</v>
+        <v>1</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B59" s="12">
-        <v>12</v>
+        <v>2006</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="12">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="12">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="5"/>
-      <c r="B62" s="12"/>
+      <c r="A62" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="12">
+        <v>24</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="A63" s="5"/>
+      <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="14">
-        <v>1.9528741509529837E-2</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>94</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="14">
+        <v>1.9528741509529837E-2</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="13">
+      <c r="B66" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="5"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>78</v>
-      </c>
+      <c r="A67" s="5"/>
+      <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B68" s="14">
-        <v>2.0648572594225215E-2</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>95</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="14">
+        <v>2.0648572594225215E-2</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="13">
+      <c r="B70" s="13">
         <v>2E-8</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="5"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B71" s="14">
-        <v>1.1841887362491711E-2</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="A71" s="5"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B72" s="14">
+        <v>1.1841887362491711E-2</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B72" s="14">
+      <c r="B73" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" s="5"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B74" s="14">
-        <v>6.2433901191501419E-2</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="A74" s="5"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" s="14">
+        <v>6.2433901191501419E-2</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B75" s="14">
+      <c r="B76" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="5"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B77" s="14">
-        <v>8.1211742157245251E-3</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="A77" s="5"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B78" s="12">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="B78" s="14">
+        <v>8.1211742157245251E-3</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D78" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" s="12">
         <v>0</v>
@@ -1809,93 +1814,93 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="12">
+        <v>0</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B80" s="12">
+      <c r="B81" s="12">
         <v>0.9</v>
       </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B81" s="12">
+      <c r="B82" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="1">
+      <c r="D82" s="2"/>
+      <c r="E82" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="5" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B82" s="12">
+      <c r="B83" s="12">
         <v>4</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83" s="5"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B84" s="12">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="A84" s="5"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B85" s="12">
-        <v>0.01</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B86" s="12">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D86" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" s="12">
         <v>0</v>
@@ -1907,100 +1912,112 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" s="12">
+        <v>0</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B88" s="12">
+      <c r="B89" s="12">
         <v>0.3</v>
       </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" s="5"/>
-      <c r="B89" s="12"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="5"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B90" s="12">
+      <c r="B91" s="12">
         <v>10</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C93" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B94" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C93" s="4"/>
-    </row>
-    <row r="94" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="5" t="s">
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B95" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B96" s="8">
-        <v>0.01</v>
-      </c>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
     </row>
     <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B97" s="8">
-        <v>3.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B98" s="8">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B99" s="8">
+      <c r="B100" s="8">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="3" t="s">
+    <row r="102" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B101" s="11"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
+      <c r="B102" s="11"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on curtailment out
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEF92F1-DE24-46FB-AD1F-7E5B10D858E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B91BA6A-90DC-441D-824D-08C0D376BC8D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21590" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1455,7 +1455,7 @@
         <v>28</v>
       </c>
       <c r="B43" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
changed input to factor form
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3F8686-CA97-4F83-9668-9171EB0ABBC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192C638B-AEFE-4631-B32A-5C1388A22212}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21590" windowHeight="7380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input - 2xNG" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="109">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>example_2xNG_1W_0.75Nuc_0.5rest_0.25PGP</t>
+  </si>
+  <si>
+    <t>example_1W_0.75Nuc_0.5rest_0.25PGP</t>
+  </si>
+  <si>
+    <t>example1</t>
   </si>
 </sst>
 </file>
@@ -1248,179 +1254,179 @@
       <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -1450,12 +1456,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -1488,12 +1494,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1515,7 +1521,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -1537,10 +1543,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
@@ -1549,10 +1555,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
@@ -1561,13 +1567,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>35</v>
       </c>
@@ -1577,7 +1583,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -1587,7 +1593,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>37</v>
       </c>
@@ -1597,7 +1603,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>38</v>
       </c>
@@ -1607,7 +1613,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1617,7 +1623,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>40</v>
       </c>
@@ -1627,7 +1633,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>41</v>
       </c>
@@ -1637,7 +1643,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
@@ -1647,13 +1653,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
@@ -1663,7 +1669,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>44</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
@@ -1690,13 +1696,13 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>47</v>
       </c>
@@ -1706,7 +1712,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -1732,13 +1738,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -1774,13 +1780,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -1806,13 +1812,13 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
@@ -1827,7 +1833,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -1839,7 +1845,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -1851,7 +1857,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -1861,7 +1867,7 @@
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -1893,13 +1899,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="12"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>99</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>100</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -1956,7 +1962,7 @@
       </c>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -1968,7 +1974,7 @@
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -1978,13 +1984,13 @@
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -1996,12 +2002,12 @@
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C93" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>66</v>
       </c>
@@ -2010,26 +2016,26 @@
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B99" s="11"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>70</v>
       </c>
@@ -2048,179 +2054,179 @@
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -2250,12 +2256,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -2277,7 +2283,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -2288,12 +2294,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -2304,7 +2310,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -2326,7 +2332,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -2337,10 +2343,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
@@ -2349,10 +2355,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
@@ -2361,13 +2367,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>35</v>
       </c>
@@ -2377,7 +2383,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -2387,7 +2393,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>37</v>
       </c>
@@ -2397,7 +2403,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>38</v>
       </c>
@@ -2407,7 +2413,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -2417,7 +2423,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>40</v>
       </c>
@@ -2427,7 +2433,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>41</v>
       </c>
@@ -2437,7 +2443,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
@@ -2447,13 +2453,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
@@ -2463,7 +2469,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>44</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
@@ -2490,13 +2496,13 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>47</v>
       </c>
@@ -2506,7 +2512,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
@@ -2520,7 +2526,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -2532,13 +2538,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -2564,13 +2570,13 @@
       </c>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -2596,13 +2602,13 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -2629,7 +2635,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -2641,7 +2647,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -2651,7 +2657,7 @@
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -2683,13 +2689,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="12"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
@@ -2704,7 +2710,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>99</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>100</v>
       </c>
@@ -2734,7 +2740,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -2746,7 +2752,7 @@
       </c>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -2758,7 +2764,7 @@
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -2768,13 +2774,13 @@
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -2786,12 +2792,12 @@
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C93" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>66</v>
       </c>
@@ -2800,26 +2806,26 @@
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B99" s="11"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>70</v>
       </c>
@@ -2838,179 +2844,179 @@
       <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -3029,7 +3035,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -3040,12 +3046,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -3056,7 +3062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -3078,12 +3084,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -3127,10 +3133,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
@@ -3139,10 +3145,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
@@ -3151,13 +3157,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>35</v>
       </c>
@@ -3167,7 +3173,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -3177,7 +3183,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>37</v>
       </c>
@@ -3187,7 +3193,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>38</v>
       </c>
@@ -3197,7 +3203,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -3207,7 +3213,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>40</v>
       </c>
@@ -3217,7 +3223,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>41</v>
       </c>
@@ -3227,7 +3233,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
@@ -3237,13 +3243,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
@@ -3253,7 +3259,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>44</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
@@ -3290,13 +3296,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>47</v>
       </c>
@@ -3306,7 +3312,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -3332,13 +3338,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -3374,13 +3380,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -3398,7 +3404,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -3414,13 +3420,13 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -3454,7 +3460,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -3469,7 +3475,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -3482,7 +3488,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>7.3048000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -3517,13 +3523,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="12"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
@@ -3542,7 +3548,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>99</v>
       </c>
@@ -3561,7 +3567,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>100</v>
       </c>
@@ -3580,7 +3586,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -3595,7 +3601,7 @@
       </c>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -3610,7 +3616,7 @@
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -3623,14 +3629,14 @@
       </c>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="12"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -3645,19 +3651,19 @@
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="5"/>
       <c r="B93" s="12"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>66</v>
       </c>
@@ -3666,26 +3672,26 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B100" s="11"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>70</v>
       </c>
@@ -3704,179 +3710,179 @@
       <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -3884,7 +3890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -3895,7 +3901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -3906,12 +3912,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -3922,7 +3928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -3933,7 +3939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -3944,12 +3950,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -3960,7 +3966,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -3982,7 +3988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -3993,10 +3999,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
@@ -4005,10 +4011,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
@@ -4017,13 +4023,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>35</v>
       </c>
@@ -4033,7 +4039,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -4043,7 +4049,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>37</v>
       </c>
@@ -4053,7 +4059,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>38</v>
       </c>
@@ -4063,7 +4069,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -4073,7 +4079,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>40</v>
       </c>
@@ -4083,7 +4089,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>41</v>
       </c>
@@ -4093,7 +4099,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
@@ -4103,13 +4109,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
@@ -4119,7 +4125,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>44</v>
       </c>
@@ -4137,7 +4143,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
@@ -4156,13 +4162,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>47</v>
       </c>
@@ -4172,7 +4178,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
@@ -4186,7 +4192,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -4198,13 +4204,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -4240,13 +4246,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -4264,7 +4270,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -4280,13 +4286,13 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
@@ -4305,7 +4311,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -4320,7 +4326,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -4335,7 +4341,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -4348,7 +4354,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -4366,7 +4372,7 @@
         <v>7.3048000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -4383,13 +4389,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="12"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
@@ -4408,7 +4414,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>99</v>
       </c>
@@ -4427,7 +4433,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>100</v>
       </c>
@@ -4446,7 +4452,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -4461,7 +4467,7 @@
       </c>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -4476,7 +4482,7 @@
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -4489,14 +4495,14 @@
       </c>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="12"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -4511,19 +4517,19 @@
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="5"/>
       <c r="B93" s="12"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>66</v>
       </c>
@@ -4532,26 +4538,26 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B100" s="11"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>70</v>
       </c>
@@ -4564,185 +4570,185 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FC5700-3688-4C40-8F9B-311966CABDFC}">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:B87"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -4750,18 +4756,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -4772,12 +4778,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -4788,7 +4794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -4799,7 +4805,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -4810,12 +4816,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -4826,7 +4832,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -4837,7 +4843,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -4848,7 +4854,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -4859,10 +4865,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
@@ -4871,10 +4877,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
@@ -4883,13 +4889,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>35</v>
       </c>
@@ -4899,7 +4905,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -4909,7 +4915,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>37</v>
       </c>
@@ -4919,7 +4925,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>38</v>
       </c>
@@ -4929,7 +4935,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -4939,7 +4945,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>40</v>
       </c>
@@ -4949,7 +4955,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>41</v>
       </c>
@@ -4959,7 +4965,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
@@ -4969,13 +4975,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
@@ -4985,13 +4991,12 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B65" s="12">
-        <f>0.5*D65</f>
-        <v>9.7643707547649186E-3</v>
+      <c r="B65" s="14">
+        <v>1.9528741509529837E-2</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>84</v>
@@ -5003,13 +5008,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B66" s="12">
-        <f>0.5*D66</f>
-        <v>5.0000000000000001E-9</v>
+      <c r="B66" s="13">
+        <f>0.00000001</f>
+        <v>1E-8</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>49</v>
@@ -5022,13 +5027,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>47</v>
       </c>
@@ -5038,7 +5043,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
@@ -5052,7 +5057,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -5064,19 +5069,18 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B72" s="14">
-        <f>2*D72</f>
-        <v>2.3683774724983422E-2</v>
+        <v>1.1841887362491711E-2</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>84</v>
@@ -5088,13 +5092,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B73" s="14">
-        <f>2*D73</f>
-        <v>4.5180018257917377E-2</v>
+        <v>2.2590009128958689E-2</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>49</v>
@@ -5106,19 +5109,18 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B75" s="12">
-        <f>0.75*D75</f>
-        <v>4.6825425893626066E-2</v>
+      <c r="B75" s="14">
+        <v>6.2433901191501419E-2</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>84</v>
@@ -5130,13 +5132,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="12">
-        <f>0.75*D76</f>
-        <v>1.8868620162126995E-2</v>
+      <c r="B76" s="14">
+        <v>2.5158160216169324E-2</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>49</v>
@@ -5146,19 +5147,19 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
-      <c r="B77" s="12"/>
+      <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B78" s="12">
-        <f>0.5*D78</f>
-        <v>1.1917808219178083E-3</v>
+        <f>261*0.08/8760</f>
+        <v>2.3835616438356165E-3</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>95</v>
@@ -5171,7 +5172,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -5186,7 +5187,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -5201,7 +5202,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -5214,7 +5215,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -5232,7 +5233,7 @@
         <v>7.3048000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -5249,19 +5250,19 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
-      <c r="B84" s="12"/>
+      <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B85" s="12">
-        <f>0.25*D85</f>
-        <v>6.8493150684931511E-7</v>
+        <f>0.3*0.08/8760</f>
+        <v>2.7397260273972604E-6</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>95</v>
@@ -5274,13 +5275,13 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B86" s="12">
-        <f t="shared" ref="B86:B87" si="0">0.25*D86</f>
-        <v>2.5114155251141552E-3</v>
+        <f>1100*0.08/8760</f>
+        <v>1.0045662100456621E-2</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>84</v>
@@ -5293,13 +5294,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B87" s="12">
-        <f t="shared" si="0"/>
-        <v>1.0502283105022832E-2</v>
+        <f>4600*0.08/8760</f>
+        <v>4.2009132420091327E-2</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>84</v>
@@ -5312,7 +5313,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -5327,7 +5328,7 @@
       </c>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -5342,7 +5343,7 @@
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -5355,14 +5356,14 @@
       </c>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="12"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -5377,19 +5378,19 @@
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="5"/>
       <c r="B93" s="12"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>66</v>
       </c>
@@ -5398,27 +5399,122 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K96" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+      <c r="B98" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C98" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D98" s="6">
+        <v>2</v>
+      </c>
+      <c r="E98" s="6">
+        <v>2</v>
+      </c>
+      <c r="F98" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="G98" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="H98" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I98" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="J98" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="K98" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C99" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D99" s="6">
+        <v>2</v>
+      </c>
+      <c r="E99" s="6">
+        <v>2</v>
+      </c>
+      <c r="F99" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="G99" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="H99" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I99" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="J99" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="K99" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B100" s="11"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="B101" s="11"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove curtailment from dispatch output
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE00E2A6-A692-4D0B-A893-7BB3016C1EF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3167F257-9125-4323-9B1B-0E15D22DA523}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21590" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,18 @@
     <sheet name="2xNG,1W,0.75nuc0.25PGP0.5rest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="119">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -376,6 +383,9 @@
   </si>
   <si>
     <t>OnlyNuclear</t>
+  </si>
+  <si>
+    <t>"BEGIN_CASE_DATA" is a keyword that must be in the first column of the file. The next row must contain keywords. Definitions here will multiply times values in  &lt;BEGIN_ALL_CASES_DATA&gt;. There must be at least one row here, because this is how the number of cases gets defined.</t>
   </si>
 </sst>
 </file>
@@ -1275,204 +1285,204 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261E599E-3D00-45DF-A9B9-819537A050D1}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.54296875" style="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="10"/>
     </row>
-    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -1480,7 +1490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -1491,7 +1501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>23</v>
       </c>
@@ -1502,12 +1512,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>26</v>
       </c>
@@ -1518,7 +1528,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>28</v>
       </c>
@@ -1529,7 +1539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>91</v>
       </c>
@@ -1540,12 +1550,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="12"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>93</v>
       </c>
@@ -1556,7 +1566,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
@@ -1567,7 +1577,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>71</v>
       </c>
@@ -1578,7 +1588,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>72</v>
       </c>
@@ -1589,10 +1599,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>32</v>
       </c>
@@ -1601,10 +1611,10 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>34</v>
       </c>
@@ -1613,13 +1623,13 @@
       </c>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="12"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +1639,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>36</v>
       </c>
@@ -1639,7 +1649,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>37</v>
       </c>
@@ -1649,7 +1659,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>38</v>
       </c>
@@ -1659,7 +1669,7 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>39</v>
       </c>
@@ -1669,7 +1679,7 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>40</v>
       </c>
@@ -1679,7 +1689,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>41</v>
       </c>
@@ -1689,7 +1699,7 @@
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>42</v>
       </c>
@@ -1699,13 +1709,13 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>43</v>
       </c>
@@ -1715,7 +1725,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>44</v>
       </c>
@@ -1729,7 +1739,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>45</v>
       </c>
@@ -1742,13 +1752,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>47</v>
       </c>
@@ -1758,7 +1768,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>48</v>
       </c>
@@ -1772,7 +1782,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>50</v>
       </c>
@@ -1784,13 +1794,13 @@
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="12"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>52</v>
       </c>
@@ -1804,7 +1814,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -1816,13 +1826,13 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="12"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>54</v>
       </c>
@@ -1836,7 +1846,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>55</v>
       </c>
@@ -1848,13 +1858,13 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="12"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>56</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>57</v>
       </c>
@@ -1881,7 +1891,7 @@
       </c>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>58</v>
       </c>
@@ -1893,7 +1903,7 @@
       </c>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>59</v>
       </c>
@@ -1903,7 +1913,7 @@
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>60</v>
       </c>
@@ -1921,7 +1931,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>63</v>
       </c>
@@ -1935,13 +1945,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="12"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>80</v>
       </c>
@@ -1956,7 +1966,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>99</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>100</v>
       </c>
@@ -1986,7 +1996,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>81</v>
       </c>
@@ -1998,7 +2008,7 @@
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>82</v>
       </c>
@@ -2010,7 +2020,7 @@
       </c>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>83</v>
       </c>
@@ -2020,13 +2030,13 @@
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="12"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>65</v>
       </c>
@@ -2038,40 +2048,40 @@
       </c>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B103" s="11"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>70</v>
       </c>
@@ -2086,204 +2096,204 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62907549-D3C5-4AC6-B75C-E35B549A753D}">
   <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.54296875" style="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="10"/>
     </row>
-    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -2291,7 +2301,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -2302,7 +2312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>23</v>
       </c>
@@ -2313,12 +2323,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>26</v>
       </c>
@@ -2329,7 +2339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>28</v>
       </c>
@@ -2340,7 +2350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>91</v>
       </c>
@@ -2351,12 +2361,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="12"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>93</v>
       </c>
@@ -2367,7 +2377,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
@@ -2378,7 +2388,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>71</v>
       </c>
@@ -2389,7 +2399,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>72</v>
       </c>
@@ -2400,10 +2410,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>32</v>
       </c>
@@ -2412,10 +2422,10 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>34</v>
       </c>
@@ -2424,13 +2434,13 @@
       </c>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="12"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>35</v>
       </c>
@@ -2440,7 +2450,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>36</v>
       </c>
@@ -2450,7 +2460,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>37</v>
       </c>
@@ -2460,7 +2470,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>38</v>
       </c>
@@ -2470,7 +2480,7 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>39</v>
       </c>
@@ -2480,7 +2490,7 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>40</v>
       </c>
@@ -2490,7 +2500,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>41</v>
       </c>
@@ -2500,7 +2510,7 @@
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>42</v>
       </c>
@@ -2510,13 +2520,13 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>43</v>
       </c>
@@ -2526,7 +2536,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>44</v>
       </c>
@@ -2540,7 +2550,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>45</v>
       </c>
@@ -2553,13 +2563,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>47</v>
       </c>
@@ -2569,7 +2579,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>48</v>
       </c>
@@ -2583,7 +2593,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>50</v>
       </c>
@@ -2595,13 +2605,13 @@
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="12"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>52</v>
       </c>
@@ -2615,7 +2625,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -2627,13 +2637,13 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="12"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>54</v>
       </c>
@@ -2647,7 +2657,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>55</v>
       </c>
@@ -2659,13 +2669,13 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="12"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>56</v>
       </c>
@@ -2680,7 +2690,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>57</v>
       </c>
@@ -2692,7 +2702,7 @@
       </c>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>58</v>
       </c>
@@ -2704,7 +2714,7 @@
       </c>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>59</v>
       </c>
@@ -2714,7 +2724,7 @@
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>60</v>
       </c>
@@ -2732,7 +2742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>63</v>
       </c>
@@ -2746,13 +2756,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="12"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>80</v>
       </c>
@@ -2767,7 +2777,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>99</v>
       </c>
@@ -2782,7 +2792,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>100</v>
       </c>
@@ -2797,7 +2807,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>81</v>
       </c>
@@ -2809,7 +2819,7 @@
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>82</v>
       </c>
@@ -2821,7 +2831,7 @@
       </c>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>83</v>
       </c>
@@ -2831,13 +2841,13 @@
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="12"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>65</v>
       </c>
@@ -2849,12 +2859,12 @@
       </c>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>66</v>
       </c>
@@ -2863,7 +2873,7 @@
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:5" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>68</v>
       </c>
@@ -2880,10 +2890,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>109</v>
       </c>
@@ -2900,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>110</v>
       </c>
@@ -2917,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>111</v>
       </c>
@@ -2934,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>112</v>
       </c>
@@ -2951,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>113</v>
       </c>
@@ -2968,7 +2978,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>114</v>
       </c>
@@ -2989,7 +2999,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
         <v>115</v>
       </c>
@@ -3010,7 +3020,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>116</v>
       </c>
@@ -3031,7 +3041,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>117</v>
       </c>
@@ -3052,13 +3062,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B111" s="11"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>70</v>
       </c>
@@ -3077,179 +3087,179 @@
       <selection activeCell="B96" sqref="B96:G96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.54296875" style="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -3257,7 +3267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -3268,7 +3278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -3279,12 +3289,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -3295,7 +3305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
@@ -3306,7 +3316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -3317,12 +3327,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -3333,7 +3343,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -3344,7 +3354,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -3355,7 +3365,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -3366,10 +3376,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
@@ -3378,10 +3388,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>34</v>
       </c>
@@ -3390,13 +3400,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>35</v>
       </c>
@@ -3406,7 +3416,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>36</v>
       </c>
@@ -3416,7 +3426,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>37</v>
       </c>
@@ -3426,7 +3436,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>38</v>
       </c>
@@ -3436,7 +3446,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -3446,7 +3456,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>40</v>
       </c>
@@ -3456,7 +3466,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>41</v>
       </c>
@@ -3466,7 +3476,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
@@ -3476,13 +3486,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>43</v>
       </c>
@@ -3492,7 +3502,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>44</v>
       </c>
@@ -3509,7 +3519,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>45</v>
       </c>
@@ -3528,13 +3538,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>47</v>
       </c>
@@ -3544,7 +3554,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
@@ -3558,7 +3568,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -3570,13 +3580,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -3593,7 +3603,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -3610,13 +3620,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -3633,7 +3643,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -3648,13 +3658,13 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
@@ -3673,7 +3683,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -3688,7 +3698,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -3703,7 +3713,7 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -3716,7 +3726,7 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -3734,7 +3744,7 @@
         <v>7.3048000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -3751,13 +3761,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
@@ -3776,7 +3786,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>99</v>
       </c>
@@ -3795,7 +3805,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>100</v>
       </c>
@@ -3814,7 +3824,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -3829,7 +3839,7 @@
       </c>
       <c r="E88" s="2"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -3844,7 +3854,7 @@
       </c>
       <c r="E89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -3857,14 +3867,14 @@
       </c>
       <c r="E90" s="2"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="12"/>
       <c r="E91" s="2"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -3879,19 +3889,19 @@
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="12"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>66</v>
       </c>
@@ -3900,7 +3910,7 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:11" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>68</v>
       </c>
@@ -3935,10 +3945,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:11" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>103</v>
       </c>
@@ -3973,7 +3983,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>104</v>
       </c>
@@ -4008,13 +4018,13 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B101" s="11"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
changed CAPACITY and DISPATCH to FIXED and VAR, respectively
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -1,35 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3167F257-9125-4323-9B1B-0E15D22DA523}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C006C-7BAE-4002-B60F-78A1530E47F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
-    <sheet name="1 gen tech at a time" sheetId="6" r:id="rId2"/>
-    <sheet name="2xNG,1W,0.75nuc0.25PGP0.5rest" sheetId="5" r:id="rId3"/>
+    <sheet name="3 days solar only gas only" sheetId="7" r:id="rId2"/>
+    <sheet name="1 gen tech at a time" sheetId="6" r:id="rId3"/>
+    <sheet name="2xNG,1W,0.75nuc0.25PGP0.5rest" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="121">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -386,6 +380,12 @@
   </si>
   <si>
     <t>"BEGIN_CASE_DATA" is a keyword that must be in the first column of the file. The next row must contain keywords. Definitions here will multiply times values in  &lt;BEGIN_ALL_CASES_DATA&gt;. There must be at least one row here, because this is how the number of cases gets defined.</t>
+  </si>
+  <si>
+    <t>3daysolarbatt</t>
+  </si>
+  <si>
+    <t>3daynatgasbatt</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261E599E-3D00-45DF-A9B9-819537A050D1}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
@@ -2093,10 +2093,875 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8DEE5D-D4A0-4BC5-A916-79B06806B187}">
+  <dimension ref="A1:F108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="10"/>
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" s="12">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="12">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="12">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="12">
+        <v>3</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" s="12">
+        <v>24</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="14">
+        <v>1.9528741509529837E-2</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" s="13">
+        <f>0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="14">
+        <v>2.0648572594225215E-2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" s="13">
+        <v>2E-8</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" s="14">
+        <v>1.1841887362491711E-2</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" s="14">
+        <v>2.2590009128958689E-2</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B79" s="14">
+        <v>6.2433901191501419E-2</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B80" s="14">
+        <v>2.5158160216169324E-2</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" s="12">
+        <f>261*0.08/8760</f>
+        <v>2.3835616438356165E-3</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83" s="12">
+        <v>0</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="12">
+        <v>0</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="1">
+        <v>7.3048000000000002E-3</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" s="12">
+        <v>6</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="12">
+        <f>0.3*0.08/8760</f>
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="12">
+        <f>1100*0.08/8760</f>
+        <v>1.0045662100456621E-2</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" s="12">
+        <f>4600*0.08/8760</f>
+        <v>4.2009132420091327E-2</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="12">
+        <v>0</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B93" s="12">
+        <v>0</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" s="12">
+        <v>10</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D101" s="6">
+        <v>-1</v>
+      </c>
+      <c r="E101" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F101" s="6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C102" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D102" s="6">
+        <v>1</v>
+      </c>
+      <c r="E102" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F102" s="6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B104" s="11"/>
+    </row>
+    <row r="108" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62907549-D3C5-4AC6-B75C-E35B549A753D}">
   <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
@@ -3079,7 +3944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FC5700-3688-4C40-8F9B-311966CABDFC}">
   <dimension ref="A1:K105"/>
   <sheetViews>

</xml_diff>

<commit_message>
changed CAPACITY and DISPATCH to FIXED and VAR in case_input.*
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C006C-7BAE-4002-B60F-78A1530E47F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B63430C-0C8C-467A-9984-DB7F0065BCDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,13 @@
     <sheet name="2xNG,1W,0.75nuc0.25PGP0.5rest" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,18 +47,12 @@
     <t>Keyword names are case insensitive.</t>
   </si>
   <si>
-    <t>To reduce errors, if one keyword exists relevant to a technology, all keywords for that technology must be defined (i.e., if you have capacity_cost_wind, you must have a dispatch_cost_wind).</t>
-  </si>
-  <si>
     <t>All energy-related (i.e., capacity) costs are in terms of $/hr per kW capacity, except for variable generators (wind and solar) it is cost per hour of deployment at the level of the associated capacity file.</t>
   </si>
   <si>
     <t>Note that costs of technologies with associated capacity files (e.g., wind solar) are assumed to be of the form where fixed costs the cost of hour of acheiveing the potential generation in the associated capacity file (i.e., there is no further normalization within the code).</t>
   </si>
   <si>
-    <t>Variable cost of energy storage (dispatch_cost_storage) is in units of $/hr per kWh stored.</t>
-  </si>
-  <si>
     <t>If the fixed cost for a technology is entered as a negative value, then that technology is assumed not to participate in the optimization.</t>
   </si>
   <si>
@@ -154,54 +155,15 @@
     <t>END_HOUR</t>
   </si>
   <si>
-    <t>SOLAR_CAPACITY_FILE</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_SOLAR</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_SOLAR</t>
-  </si>
-  <si>
     <t>The idea is that this should be a small number, and smaller than wind, so solar is curtailed first</t>
   </si>
   <si>
-    <t>WIND_CAPACITY_FILE</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_WIND</t>
-  </si>
-  <si>
     <t>$/kWh</t>
   </si>
   <si>
-    <t>DISPATCH_COST_WIND</t>
-  </si>
-  <si>
     <t>The idea is that this should be a small number, but bigger than solar, so solar is curtailed first</t>
   </si>
   <si>
-    <t>CAPACITY_COST_NATGAS</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_NATGAS</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_NUCLEAR</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_NUCLEAR</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_TO_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_FROM_STORAGE</t>
-  </si>
-  <si>
     <t>STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
@@ -220,9 +182,6 @@
     <t>hours</t>
   </si>
   <si>
-    <t>DISPATCH_COST_UNMET_DEMAND</t>
-  </si>
-  <si>
     <t>BEGIN_CASE_DATA</t>
   </si>
   <si>
@@ -265,15 +224,6 @@
     <t>demand_series_Shaner_normalized_to_1_mean.csv</t>
   </si>
   <si>
-    <t>CAPACITY_COST_PGP_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_TO_PGP_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_FROM_PGP_STORAGE</t>
-  </si>
-  <si>
     <t>PGP_STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
@@ -322,12 +272,6 @@
     <t>2.7e-6 adds on about 2.4 cents per kWh if used one cycle per year</t>
   </si>
   <si>
-    <t>CAPACITY_COST_TO_PGP_STORAGE</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_FROM_PGP_STORAGE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electrolyser $4600 per kW capital cost. Assume 8% capital recovery factor and 8760 hours per year = </t>
   </si>
   <si>
@@ -386,6 +330,69 @@
   </si>
   <si>
     <t>3daynatgasbatt</t>
+  </si>
+  <si>
+    <t>SOLAR_FIXED_FILE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_SOLAR</t>
+  </si>
+  <si>
+    <t>WIND_FIXED_FILE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_WIND</t>
+  </si>
+  <si>
+    <t>FIXED_COST_NATGAS</t>
+  </si>
+  <si>
+    <t>FIXED_COST_NUCLEAR</t>
+  </si>
+  <si>
+    <t>FIXED_COST_STORAGE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_TO_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_FROM_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>To reduce errors, if one keyword exists relevant to a technology, all keywords for that technology must be defined (i.e., if you have FIXED_cost_wind, you must have a VAR_cost_wind).</t>
+  </si>
+  <si>
+    <t>Variable cost of energy storage (VAR_cost_storage) is in units of $/hr per kWh stored.</t>
+  </si>
+  <si>
+    <t>VAR_COST_SOLAR</t>
+  </si>
+  <si>
+    <t>VAR_COST_WIND</t>
+  </si>
+  <si>
+    <t>VAR_COST_NATGAS</t>
+  </si>
+  <si>
+    <t>VAR_COST_NUCLEAR</t>
+  </si>
+  <si>
+    <t>VAR_COST_TO_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_FROM_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_TO_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_FROM_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_UNMET_DEMAND</t>
   </si>
 </sst>
 </file>
@@ -1316,19 +1323,19 @@
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -1358,7 +1365,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -1367,7 +1374,7 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="10"/>
     </row>
@@ -1376,7 +1383,7 @@
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="10"/>
     </row>
@@ -1385,13 +1392,13 @@
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -1400,7 +1407,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -1409,7 +1416,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -1418,7 +1425,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -1427,7 +1434,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -1436,7 +1443,7 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -1445,7 +1452,7 @@
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="10"/>
     </row>
@@ -1454,13 +1461,13 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="10"/>
     </row>
@@ -1469,7 +1476,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="10"/>
     </row>
@@ -1478,38 +1485,38 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="10"/>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,35 +1526,35 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B48" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,46 +1564,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B50" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B52" s="13">
         <v>1000000000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B53" s="13">
         <v>1000000000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,10 +1611,10 @@
     </row>
     <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
     </row>
@@ -1616,10 +1623,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -1631,7 +1638,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -1641,7 +1648,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="12">
         <v>1</v>
@@ -1651,7 +1658,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B61" s="12">
         <v>1</v>
@@ -1661,7 +1668,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="12">
         <v>1</v>
@@ -1671,7 +1678,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="12">
         <v>2006</v>
@@ -1681,7 +1688,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B64" s="12">
         <v>12</v>
@@ -1691,7 +1698,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12">
         <v>31</v>
@@ -1701,7 +1708,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="12">
         <v>24</v>
@@ -1717,38 +1724,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="B69" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="B70" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -1760,37 +1767,37 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="B73" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B74" s="13">
         <v>2E-8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -1802,27 +1809,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B76" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B77" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -1834,27 +1841,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B79" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B80" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -1866,46 +1873,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B82" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B83" s="12">
         <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B84" s="12">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B85" s="12">
         <v>0.9</v>
@@ -1915,34 +1922,34 @@
     </row>
     <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B86" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,76 +1960,76 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B89" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B90" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B91" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="B92" s="12">
         <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B93" s="12">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B94" s="12">
         <v>0.3</v>
@@ -2038,33 +2045,33 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B96" s="12">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2072,18 +2079,18 @@
     </row>
     <row r="101" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B103" s="11"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2127,19 +2134,19 @@
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -2169,7 +2176,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -2178,7 +2185,7 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="10"/>
     </row>
@@ -2187,7 +2194,7 @@
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="10"/>
     </row>
@@ -2196,13 +2203,13 @@
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -2211,7 +2218,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -2220,7 +2227,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -2229,7 +2236,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -2238,7 +2245,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -2247,7 +2254,7 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -2256,7 +2263,7 @@
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="10"/>
     </row>
@@ -2265,13 +2272,13 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="10"/>
     </row>
@@ -2280,7 +2287,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="10"/>
     </row>
@@ -2289,38 +2296,38 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="10"/>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2330,35 +2337,35 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B48" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,46 +2375,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B50" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B52" s="13">
         <v>1000000000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B53" s="13">
         <v>1000000000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2415,10 +2422,10 @@
     </row>
     <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
     </row>
@@ -2427,10 +2434,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -2442,7 +2449,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -2452,7 +2459,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="12">
         <v>1</v>
@@ -2462,7 +2469,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B61" s="12">
         <v>1</v>
@@ -2472,7 +2479,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="12">
         <v>1</v>
@@ -2482,7 +2489,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="12">
         <v>2006</v>
@@ -2492,7 +2499,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B64" s="12">
         <v>1</v>
@@ -2502,7 +2509,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12">
         <v>3</v>
@@ -2512,7 +2519,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="12">
         <v>24</v>
@@ -2528,38 +2535,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="B69" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="B70" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -2571,37 +2578,37 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="B73" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B74" s="13">
         <v>2E-8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -2613,27 +2620,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B76" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B77" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -2645,27 +2652,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B79" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B80" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -2677,46 +2684,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B82" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B83" s="12">
         <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B84" s="12">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B85" s="12">
         <v>0.9</v>
@@ -2726,34 +2733,34 @@
     </row>
     <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B86" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,76 +2771,76 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B89" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B90" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B91" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="B92" s="12">
         <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B93" s="12">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B94" s="12">
         <v>0.3</v>
@@ -2849,48 +2856,48 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B96" s="12">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2898,7 +2905,7 @@
     </row>
     <row r="101" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B101" s="6">
         <v>1</v>
@@ -2918,7 +2925,7 @@
     </row>
     <row r="102" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B102" s="6">
         <v>-1</v>
@@ -2938,13 +2945,13 @@
     </row>
     <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B104" s="11"/>
     </row>
     <row r="108" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -2992,19 +2999,19 @@
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -3034,7 +3041,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -3043,7 +3050,7 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="10"/>
     </row>
@@ -3052,7 +3059,7 @@
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="10"/>
     </row>
@@ -3061,13 +3068,13 @@
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -3076,7 +3083,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -3085,7 +3092,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -3094,7 +3101,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -3103,7 +3110,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -3112,7 +3119,7 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -3121,7 +3128,7 @@
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="10"/>
     </row>
@@ -3130,13 +3137,13 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="10"/>
     </row>
@@ -3145,7 +3152,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="10"/>
     </row>
@@ -3154,38 +3161,38 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="10"/>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,35 +3202,35 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B48" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,46 +3240,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B50" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B52" s="13">
         <v>1000000000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B53" s="13">
         <v>1000000000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3280,10 +3287,10 @@
     </row>
     <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
     </row>
@@ -3292,10 +3299,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -3307,7 +3314,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -3317,7 +3324,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="12">
         <v>1</v>
@@ -3327,7 +3334,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B61" s="12">
         <v>1</v>
@@ -3337,7 +3344,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="12">
         <v>1</v>
@@ -3347,7 +3354,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="12">
         <v>2006</v>
@@ -3357,7 +3364,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B64" s="12">
         <v>12</v>
@@ -3367,7 +3374,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12">
         <v>31</v>
@@ -3377,7 +3384,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="12">
         <v>24</v>
@@ -3393,38 +3400,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="B69" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="B70" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -3436,37 +3443,37 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="B73" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B74" s="13">
         <v>2E-8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -3478,27 +3485,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B76" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B77" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -3510,27 +3517,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B79" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B80" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -3542,46 +3549,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B82" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B83" s="12">
         <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B84" s="12">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B85" s="12">
         <v>0.9</v>
@@ -3591,34 +3598,34 @@
     </row>
     <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B86" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3629,76 +3636,76 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B89" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B90" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B91" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="B92" s="12">
         <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B93" s="12">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B94" s="12">
         <v>0.3</v>
@@ -3714,45 +3721,45 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B96" s="12">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3760,7 +3767,7 @@
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B101" s="6">
         <v>1</v>
@@ -3777,7 +3784,7 @@
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="B102" s="6">
         <v>-1</v>
@@ -3794,7 +3801,7 @@
     </row>
     <row r="103" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B103" s="6">
         <v>1</v>
@@ -3811,7 +3818,7 @@
     </row>
     <row r="104" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="B104" s="6">
         <v>1</v>
@@ -3828,7 +3835,7 @@
     </row>
     <row r="105" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B105" s="6">
         <v>1</v>
@@ -3845,7 +3852,7 @@
     </row>
     <row r="106" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B106" s="6">
         <f>-1*B102</f>
@@ -3866,7 +3873,7 @@
     </row>
     <row r="107" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B107" s="6">
         <f t="shared" ref="B107:E107" si="1">-1*B103</f>
@@ -3887,7 +3894,7 @@
     </row>
     <row r="108" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B108" s="6">
         <f t="shared" ref="B108:E108" si="2">-1*B104</f>
@@ -3908,7 +3915,7 @@
     </row>
     <row r="109" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B109" s="6">
         <f t="shared" ref="B109:E109" si="3">-1*B105</f>
@@ -3929,13 +3936,13 @@
     </row>
     <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B111" s="11"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4000,7 +4007,7 @@
     </row>
     <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B9" s="10"/>
     </row>
@@ -4009,7 +4016,7 @@
     </row>
     <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="10"/>
     </row>
@@ -4018,7 +4025,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -4027,13 +4034,13 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="B16" s="10"/>
     </row>
@@ -4042,7 +4049,7 @@
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="10"/>
     </row>
@@ -4051,7 +4058,7 @@
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -4060,7 +4067,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -4069,7 +4076,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -4078,7 +4085,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -4087,7 +4094,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -4096,13 +4103,13 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="10"/>
     </row>
     <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="10"/>
     </row>
@@ -4111,7 +4118,7 @@
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="10"/>
     </row>
@@ -4120,38 +4127,38 @@
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B35" s="10"/>
     </row>
     <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4161,35 +4168,35 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B43" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B44" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4199,46 +4206,46 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B48" s="13">
         <v>1000000000</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B49" s="13">
         <v>1000000000</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4246,10 +4253,10 @@
     </row>
     <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51" s="4"/>
     </row>
@@ -4258,10 +4265,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C53" s="2"/>
     </row>
@@ -4273,7 +4280,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B55" s="12">
         <v>2006</v>
@@ -4283,7 +4290,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B56" s="12">
         <v>1</v>
@@ -4293,7 +4300,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B57" s="12">
         <v>1</v>
@@ -4303,7 +4310,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B58" s="12">
         <v>1</v>
@@ -4313,7 +4320,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -4323,7 +4330,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B60" s="12">
         <v>12</v>
@@ -4333,7 +4340,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B61" s="12">
         <v>31</v>
@@ -4343,7 +4350,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B62" s="12">
         <v>24</v>
@@ -4359,48 +4366,48 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="B65" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D65" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="B66" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D66" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4411,37 +4418,37 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="B69" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B70" s="13">
         <v>2E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -4453,36 +4460,36 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B72" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D72" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B73" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D73" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4493,30 +4500,30 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B75" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D75" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B76" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D76" s="14">
         <v>2.5158160216169324E-2</v>
@@ -4531,32 +4538,32 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B78" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D78" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B79" s="12">
         <v>0</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D79" s="12">
         <v>0</v>
@@ -4565,13 +4572,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B80" s="12">
         <v>0</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D80" s="12">
         <v>0</v>
@@ -4580,7 +4587,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B81" s="12">
         <v>0.9</v>
@@ -4593,13 +4600,13 @@
     </row>
     <row r="82" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B82" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D82" s="12">
         <v>1.0000000000000001E-5</v>
@@ -4611,19 +4618,19 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B83" s="12">
         <v>6</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D83" s="12">
         <v>6</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -4634,70 +4641,70 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B85" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D85" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B86" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D86" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B87" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D87" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="B88" s="12">
         <v>0</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D88" s="12">
         <v>0</v>
@@ -4706,13 +4713,13 @@
     </row>
     <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B89" s="12">
         <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D89" s="12">
         <v>0</v>
@@ -4721,7 +4728,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B90" s="12">
         <v>0.3</v>
@@ -4741,13 +4748,13 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="B92" s="12">
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D92" s="12">
         <v>10</v>
@@ -4763,51 +4770,51 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C94" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C95" s="4"/>
     </row>
     <row r="96" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4815,7 +4822,7 @@
     </row>
     <row r="98" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B98" s="6">
         <v>0.5</v>
@@ -4850,7 +4857,7 @@
     </row>
     <row r="99" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B99" s="6">
         <v>-1</v>
@@ -4885,13 +4892,13 @@
     </row>
     <row r="101" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B101" s="11"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on cost model
</commit_message>
<xml_diff>
--- a/case_input.xlsx
+++ b/case_input.xlsx
@@ -8,22 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C006C-7BAE-4002-B60F-78A1530E47F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D245555D-7A65-47A9-83C6-004ED2E8918B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
-    <sheet name="3 days solar only gas only" sheetId="7" r:id="rId2"/>
-    <sheet name="1 gen tech at a time" sheetId="6" r:id="rId3"/>
-    <sheet name="2xNG,1W,0.75nuc0.25PGP0.5rest" sheetId="5" r:id="rId4"/>
+    <sheet name="tweaktest" sheetId="8" r:id="rId2"/>
+    <sheet name="3 days solar only gas only" sheetId="7" r:id="rId3"/>
+    <sheet name="1 gen tech at a time" sheetId="6" r:id="rId4"/>
+    <sheet name="2xNG,1W,0.75nuc0.25PGP0.5rest" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="126">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -40,18 +48,12 @@
     <t>Keyword names are case insensitive.</t>
   </si>
   <si>
-    <t>To reduce errors, if one keyword exists relevant to a technology, all keywords for that technology must be defined (i.e., if you have capacity_cost_wind, you must have a dispatch_cost_wind).</t>
-  </si>
-  <si>
     <t>All energy-related (i.e., capacity) costs are in terms of $/hr per kW capacity, except for variable generators (wind and solar) it is cost per hour of deployment at the level of the associated capacity file.</t>
   </si>
   <si>
     <t>Note that costs of technologies with associated capacity files (e.g., wind solar) are assumed to be of the form where fixed costs the cost of hour of acheiveing the potential generation in the associated capacity file (i.e., there is no further normalization within the code).</t>
   </si>
   <si>
-    <t>Variable cost of energy storage (dispatch_cost_storage) is in units of $/hr per kWh stored.</t>
-  </si>
-  <si>
     <t>If the fixed cost for a technology is entered as a negative value, then that technology is assumed not to participate in the optimization.</t>
   </si>
   <si>
@@ -157,51 +159,18 @@
     <t>SOLAR_CAPACITY_FILE</t>
   </si>
   <si>
-    <t>CAPACITY_COST_SOLAR</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_SOLAR</t>
-  </si>
-  <si>
     <t>The idea is that this should be a small number, and smaller than wind, so solar is curtailed first</t>
   </si>
   <si>
     <t>WIND_CAPACITY_FILE</t>
   </si>
   <si>
-    <t>CAPACITY_COST_WIND</t>
-  </si>
-  <si>
     <t>$/kWh</t>
   </si>
   <si>
-    <t>DISPATCH_COST_WIND</t>
-  </si>
-  <si>
     <t>The idea is that this should be a small number, but bigger than solar, so solar is curtailed first</t>
   </si>
   <si>
-    <t>CAPACITY_COST_NATGAS</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_NATGAS</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_NUCLEAR</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_NUCLEAR</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_TO_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_FROM_STORAGE</t>
-  </si>
-  <si>
     <t>STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
@@ -220,9 +189,6 @@
     <t>hours</t>
   </si>
   <si>
-    <t>DISPATCH_COST_UNMET_DEMAND</t>
-  </si>
-  <si>
     <t>BEGIN_CASE_DATA</t>
   </si>
   <si>
@@ -265,15 +231,6 @@
     <t>demand_series_Shaner_normalized_to_1_mean.csv</t>
   </si>
   <si>
-    <t>CAPACITY_COST_PGP_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_TO_PGP_STORAGE</t>
-  </si>
-  <si>
-    <t>DISPATCH_COST_FROM_PGP_STORAGE</t>
-  </si>
-  <si>
     <t>PGP_STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
@@ -322,12 +279,6 @@
     <t>2.7e-6 adds on about 2.4 cents per kWh if used one cycle per year</t>
   </si>
   <si>
-    <t>CAPACITY_COST_TO_PGP_STORAGE</t>
-  </si>
-  <si>
-    <t>CAPACITY_COST_FROM_PGP_STORAGE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electrolyser $4600 per kW capital cost. Assume 8% capital recovery factor and 8760 hours per year = </t>
   </si>
   <si>
@@ -386,6 +337,78 @@
   </si>
   <si>
     <t>3daynatgasbatt</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>Variable cost of energy storage (VAR_COST_storage) is in units of $/hr per kWh stored.</t>
+  </si>
+  <si>
+    <t>VAR_COST_SOLAR</t>
+  </si>
+  <si>
+    <t>VAR_COST_WIND</t>
+  </si>
+  <si>
+    <t>VAR_COST_NATGAS</t>
+  </si>
+  <si>
+    <t>VAR_COST_NUCLEAR</t>
+  </si>
+  <si>
+    <t>VAR_COST_TO_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_FROM_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_TO_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_FROM_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>VAR_COST_UNMET_DEMAND</t>
+  </si>
+  <si>
+    <t>To reduce errors, if one keyword exists relevant to a technology, all keywords for that technology must be defined (i.e., if you have FIXED_COST_wind, you must have a VAR_COST_wind).</t>
+  </si>
+  <si>
+    <t>FIXED_COST_SOLAR</t>
+  </si>
+  <si>
+    <t>FIXED_COST_WIND</t>
+  </si>
+  <si>
+    <t>FIXED_COST_NATGAS</t>
+  </si>
+  <si>
+    <t>FIXED_COST_NUCLEAR</t>
+  </si>
+  <si>
+    <t>FIXED_COST_STORAGE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_TO_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>FIXED_COST_FROM_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test0</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261E599E-3D00-45DF-A9B9-819537A050D1}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:R108"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="Q98" sqref="Q98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,19 +1339,19 @@
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -1358,7 +1381,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -1367,7 +1390,7 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="10"/>
     </row>
@@ -1376,7 +1399,7 @@
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="10"/>
     </row>
@@ -1385,13 +1408,13 @@
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -1400,7 +1423,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -1409,7 +1432,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -1418,7 +1441,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -1427,7 +1450,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -1436,7 +1459,7 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -1445,7 +1468,7 @@
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="10"/>
     </row>
@@ -1454,13 +1477,13 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="10"/>
     </row>
@@ -1469,7 +1492,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="10"/>
     </row>
@@ -1478,38 +1501,38 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="10"/>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,35 +1542,35 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B48" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,46 +1580,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B50" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B52" s="13">
         <v>1000000000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B53" s="13">
         <v>1000000000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,10 +1627,10 @@
     </row>
     <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
     </row>
@@ -1616,10 +1639,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -1631,7 +1654,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -1641,7 +1664,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="12">
         <v>1</v>
@@ -1651,7 +1674,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B61" s="12">
         <v>1</v>
@@ -1661,7 +1684,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="12">
         <v>1</v>
@@ -1671,7 +1694,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="12">
         <v>2006</v>
@@ -1681,7 +1704,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B64" s="12">
         <v>12</v>
@@ -1691,7 +1714,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12">
         <v>31</v>
@@ -1701,7 +1724,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="12">
         <v>24</v>
@@ -1717,38 +1740,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B69" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B70" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -1760,37 +1783,37 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B73" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B74" s="13">
         <v>2E-8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -1802,27 +1825,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B76" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B77" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -1834,27 +1857,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B79" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B80" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -1866,46 +1889,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="B82" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B83" s="12">
         <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="B84" s="12">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B85" s="12">
         <v>0.9</v>
@@ -1915,34 +1938,34 @@
     </row>
     <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B86" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,76 +1976,76 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="B89" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B90" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B91" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B92" s="12">
         <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B93" s="12">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B94" s="12">
         <v>0.3</v>
@@ -2038,52 +2061,210 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B96" s="12">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B98" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="1:18" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J99" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C98" s="4"/>
-    </row>
-    <row r="99" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K99" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L99" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M99" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N99" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="O99" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="P99" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q99" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="R99" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B103" s="11"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>70</v>
+        <v>102</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6">
+        <v>1</v>
+      </c>
+      <c r="D101" s="6">
+        <v>1</v>
+      </c>
+      <c r="E101" s="6">
+        <v>1</v>
+      </c>
+      <c r="F101" s="6">
+        <v>1</v>
+      </c>
+      <c r="G101" s="6">
+        <v>1</v>
+      </c>
+      <c r="H101" s="6">
+        <v>1</v>
+      </c>
+      <c r="I101" s="6">
+        <v>1</v>
+      </c>
+      <c r="J101" s="6">
+        <v>1</v>
+      </c>
+      <c r="K101" s="6">
+        <v>1</v>
+      </c>
+      <c r="L101" s="6">
+        <v>1</v>
+      </c>
+      <c r="M101" s="6">
+        <v>1</v>
+      </c>
+      <c r="N101" s="6">
+        <v>1</v>
+      </c>
+      <c r="O101" s="6">
+        <v>1</v>
+      </c>
+      <c r="P101" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q101" s="6">
+        <v>1</v>
+      </c>
+      <c r="R101" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B102" s="6">
+        <v>1</v>
+      </c>
+      <c r="C102" s="6">
+        <v>1</v>
+      </c>
+      <c r="D102" s="6">
+        <v>1</v>
+      </c>
+      <c r="E102" s="6">
+        <v>1</v>
+      </c>
+      <c r="F102" s="6">
+        <v>2</v>
+      </c>
+      <c r="G102" s="6">
+        <v>2</v>
+      </c>
+      <c r="H102" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="I102" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="J102" s="6">
+        <v>1</v>
+      </c>
+      <c r="K102" s="6">
+        <v>1</v>
+      </c>
+      <c r="L102" s="6">
+        <v>1</v>
+      </c>
+      <c r="M102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="P102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Q102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R102" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B104" s="11"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2093,10 +2274,1097 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAB1EB0-472A-4DD0-9E69-6F84B61B7AD5}">
+  <dimension ref="A1:R109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="10"/>
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="12">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62" s="12">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="12">
+        <v>12</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="12">
+        <v>31</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" s="12">
+        <v>24</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="14">
+        <v>1.9528741509529837E-2</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" s="13">
+        <f>0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" s="14">
+        <v>2.0648572594225215E-2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="13">
+        <v>2E-8</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" s="14">
+        <v>1.1841887362491711E-2</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B77" s="14">
+        <v>2.2590009128958689E-2</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="14">
+        <v>6.2433901191501419E-2</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80" s="14">
+        <v>2.5158160216169324E-2</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="12">
+        <f>261*0.08/8760</f>
+        <v>2.3835616438356165E-3</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B83" s="12">
+        <v>0</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" s="12">
+        <v>0</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B86" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="1">
+        <v>7.3048000000000002E-3</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B87" s="12">
+        <v>6</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" s="12">
+        <f>0.3*0.08/8760</f>
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B90" s="12">
+        <f>1100*0.08/8760</f>
+        <v>1.0045662100456621E-2</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B91" s="12">
+        <f>4600*0.08/8760</f>
+        <v>4.2009132420091327E-2</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B92" s="12">
+        <v>0</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" s="12">
+        <v>0</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B96" s="12">
+        <v>10</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="1:18" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K99" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L99" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M99" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N99" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="O99" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="P99" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q99" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="R99" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6">
+        <v>1</v>
+      </c>
+      <c r="D101" s="6">
+        <v>1</v>
+      </c>
+      <c r="E101" s="6">
+        <v>1</v>
+      </c>
+      <c r="F101" s="6">
+        <f>2*0.8/0.75</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="G101" s="6">
+        <f>2*0.8/0.75</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="H101" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="I101" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="J101" s="6">
+        <v>1</v>
+      </c>
+      <c r="K101" s="6">
+        <v>1</v>
+      </c>
+      <c r="L101" s="6">
+        <v>1</v>
+      </c>
+      <c r="M101" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N101" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O101" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="P101" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Q101" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R101" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B102" s="6">
+        <v>1</v>
+      </c>
+      <c r="C102" s="6">
+        <v>1</v>
+      </c>
+      <c r="D102" s="6">
+        <v>1</v>
+      </c>
+      <c r="E102" s="6">
+        <v>1</v>
+      </c>
+      <c r="F102" s="6">
+        <f>2*0.85/0.75</f>
+        <v>2.2666666666666666</v>
+      </c>
+      <c r="G102" s="6">
+        <f>2*0.85/0.75</f>
+        <v>2.2666666666666666</v>
+      </c>
+      <c r="H102" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I102" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="J102" s="6">
+        <v>1</v>
+      </c>
+      <c r="K102" s="6">
+        <v>1</v>
+      </c>
+      <c r="L102" s="6">
+        <v>1</v>
+      </c>
+      <c r="M102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="P102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Q102" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R102" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103" s="6">
+        <v>1</v>
+      </c>
+      <c r="D103" s="6">
+        <v>1</v>
+      </c>
+      <c r="E103" s="6">
+        <v>1</v>
+      </c>
+      <c r="F103" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G103" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H103" s="6">
+        <f>0.75*F103/2</f>
+        <v>0.9375</v>
+      </c>
+      <c r="I103" s="6">
+        <f>0.75*G103/2</f>
+        <v>0.9375</v>
+      </c>
+      <c r="J103" s="6">
+        <v>1</v>
+      </c>
+      <c r="K103" s="6">
+        <v>1</v>
+      </c>
+      <c r="L103" s="6">
+        <v>1</v>
+      </c>
+      <c r="M103" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N103" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="O103" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="P103" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Q103" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R103" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105" s="11"/>
+    </row>
+    <row r="107" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="6">
+        <v>1</v>
+      </c>
+      <c r="C107" s="6">
+        <v>1</v>
+      </c>
+      <c r="D107" s="6">
+        <v>1</v>
+      </c>
+      <c r="E107" s="6">
+        <v>1</v>
+      </c>
+      <c r="F107" s="6">
+        <v>1</v>
+      </c>
+      <c r="G107" s="6">
+        <v>1</v>
+      </c>
+      <c r="H107" s="6">
+        <v>1</v>
+      </c>
+      <c r="I107" s="6">
+        <v>1</v>
+      </c>
+      <c r="J107" s="6">
+        <v>1</v>
+      </c>
+      <c r="K107" s="6">
+        <v>1</v>
+      </c>
+      <c r="L107" s="6">
+        <v>1</v>
+      </c>
+      <c r="M107" s="6">
+        <v>1</v>
+      </c>
+      <c r="N107" s="6">
+        <v>1</v>
+      </c>
+      <c r="O107" s="6">
+        <v>1</v>
+      </c>
+      <c r="P107" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q107" s="6">
+        <v>1</v>
+      </c>
+      <c r="R107" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8DEE5D-D4A0-4BC5-A916-79B06806B187}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
@@ -2127,19 +3395,19 @@
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -2169,7 +3437,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -2178,7 +3446,7 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="10"/>
     </row>
@@ -2187,7 +3455,7 @@
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="10"/>
     </row>
@@ -2196,13 +3464,13 @@
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -2211,7 +3479,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -2220,7 +3488,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -2229,7 +3497,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -2238,7 +3506,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -2247,7 +3515,7 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -2256,7 +3524,7 @@
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="10"/>
     </row>
@@ -2265,13 +3533,13 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="10"/>
     </row>
@@ -2280,7 +3548,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="10"/>
     </row>
@@ -2289,38 +3557,38 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="10"/>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2330,35 +3598,35 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B48" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,46 +3636,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B50" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B52" s="13">
         <v>1000000000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B53" s="13">
         <v>1000000000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2415,10 +3683,10 @@
     </row>
     <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
     </row>
@@ -2427,10 +3695,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -2442,7 +3710,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -2452,7 +3720,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="12">
         <v>1</v>
@@ -2462,7 +3730,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B61" s="12">
         <v>1</v>
@@ -2472,7 +3740,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="12">
         <v>1</v>
@@ -2482,7 +3750,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="12">
         <v>2006</v>
@@ -2492,7 +3760,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B64" s="12">
         <v>1</v>
@@ -2502,7 +3770,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12">
         <v>3</v>
@@ -2512,7 +3780,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="12">
         <v>24</v>
@@ -2528,38 +3796,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B69" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B70" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -2571,37 +3839,37 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B73" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B74" s="13">
         <v>2E-8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -2613,27 +3881,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B76" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B77" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -2645,27 +3913,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B79" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B80" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -2677,46 +3945,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="B82" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B83" s="12">
         <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="B84" s="12">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B85" s="12">
         <v>0.9</v>
@@ -2726,34 +3994,34 @@
     </row>
     <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B86" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,76 +4032,76 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="B89" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B90" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B91" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B92" s="12">
         <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B93" s="12">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B94" s="12">
         <v>0.3</v>
@@ -2849,48 +4117,48 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B96" s="12">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2898,7 +4166,7 @@
     </row>
     <row r="101" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B101" s="6">
         <v>1</v>
@@ -2918,7 +4186,7 @@
     </row>
     <row r="102" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B102" s="6">
         <v>-1</v>
@@ -2938,13 +4206,13 @@
     </row>
     <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B104" s="11"/>
     </row>
     <row r="108" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -2957,7 +4225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62907549-D3C5-4AC6-B75C-E35B549A753D}">
   <dimension ref="A1:F115"/>
   <sheetViews>
@@ -2992,19 +4260,19 @@
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -3034,7 +4302,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -3043,7 +4311,7 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="10"/>
     </row>
@@ -3052,7 +4320,7 @@
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="10"/>
     </row>
@@ -3061,13 +4329,13 @@
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -3076,7 +4344,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -3085,7 +4353,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -3094,7 +4362,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -3103,7 +4371,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -3112,7 +4380,7 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="10"/>
     </row>
@@ -3121,7 +4389,7 @@
     </row>
     <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" s="10"/>
     </row>
@@ -3130,13 +4398,13 @@
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="10"/>
     </row>
@@ -3145,7 +4413,7 @@
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" s="10"/>
     </row>
@@ -3154,38 +4422,38 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39" s="10"/>
     </row>
     <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,35 +4463,35 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B48" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,46 +4501,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B50" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B52" s="13">
         <v>1000000000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B53" s="13">
         <v>1000000000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3280,10 +4548,10 @@
     </row>
     <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
     </row>
@@ -3292,10 +4560,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -3307,7 +4575,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -3317,7 +4585,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B60" s="12">
         <v>1</v>
@@ -3327,7 +4595,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B61" s="12">
         <v>1</v>
@@ -3337,7 +4605,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="12">
         <v>1</v>
@@ -3347,7 +4615,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="12">
         <v>2006</v>
@@ -3357,7 +4625,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B64" s="12">
         <v>12</v>
@@ -3367,7 +4635,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" s="12">
         <v>31</v>
@@ -3377,7 +4645,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="12">
         <v>24</v>
@@ -3393,38 +4661,38 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B69" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B70" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -3436,37 +4704,37 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B73" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B74" s="13">
         <v>2E-8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -3478,27 +4746,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B76" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B77" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -3510,27 +4778,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B79" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B80" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -3542,46 +4810,46 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="B82" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B83" s="12">
         <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="B84" s="12">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B85" s="12">
         <v>0.9</v>
@@ -3591,34 +4859,34 @@
     </row>
     <row r="86" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B86" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="1">
         <v>7.3048000000000002E-3</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B87" s="12">
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3629,76 +4897,76 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="B89" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B90" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B91" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B92" s="12">
         <v>0</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B93" s="12">
         <v>0</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B94" s="12">
         <v>0.3</v>
@@ -3714,45 +4982,45 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B96" s="12">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3760,7 +5028,7 @@
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B101" s="6">
         <v>1</v>
@@ -3777,7 +5045,7 @@
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="B102" s="6">
         <v>-1</v>
@@ -3794,7 +5062,7 @@
     </row>
     <row r="103" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B103" s="6">
         <v>1</v>
@@ -3811,7 +5079,7 @@
     </row>
     <row r="104" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B104" s="6">
         <v>1</v>
@@ -3828,7 +5096,7 @@
     </row>
     <row r="105" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B105" s="6">
         <v>1</v>
@@ -3845,7 +5113,7 @@
     </row>
     <row r="106" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B106" s="6">
         <f>-1*B102</f>
@@ -3866,7 +5134,7 @@
     </row>
     <row r="107" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B107" s="6">
         <f t="shared" ref="B107:E107" si="1">-1*B103</f>
@@ -3887,7 +5155,7 @@
     </row>
     <row r="108" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B108" s="6">
         <f t="shared" ref="B108:E108" si="2">-1*B104</f>
@@ -3908,7 +5176,7 @@
     </row>
     <row r="109" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B109" s="6">
         <f t="shared" ref="B109:E109" si="3">-1*B105</f>
@@ -3929,13 +5197,13 @@
     </row>
     <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B111" s="11"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3944,7 +5212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FC5700-3688-4C40-8F9B-311966CABDFC}">
   <dimension ref="A1:K105"/>
   <sheetViews>
@@ -4000,7 +5268,7 @@
     </row>
     <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B9" s="10"/>
     </row>
@@ -4009,7 +5277,7 @@
     </row>
     <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="10"/>
     </row>
@@ -4018,7 +5286,7 @@
     </row>
     <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="10"/>
     </row>
@@ -4027,13 +5295,13 @@
     </row>
     <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="B16" s="10"/>
     </row>
@@ -4042,7 +5310,7 @@
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="10"/>
     </row>
@@ -4051,7 +5319,7 @@
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="10"/>
     </row>
@@ -4060,7 +5328,7 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" s="10"/>
     </row>
@@ -4069,7 +5337,7 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="10"/>
     </row>
@@ -4078,7 +5346,7 @@
     </row>
     <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="10"/>
     </row>
@@ -4087,7 +5355,7 @@
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="10"/>
     </row>
@@ -4096,13 +5364,13 @@
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="10"/>
     </row>
     <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="10"/>
     </row>
@@ -4111,7 +5379,7 @@
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="10"/>
     </row>
@@ -4120,38 +5388,38 @@
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B35" s="10"/>
     </row>
     <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4161,35 +5429,35 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B42" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B43" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B44" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4199,46 +5467,46 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B48" s="13">
         <v>1000000000</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B49" s="13">
         <v>1000000000</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4246,10 +5514,10 @@
     </row>
     <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51" s="4"/>
     </row>
@@ -4258,10 +5526,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2"/>
     </row>
@@ -4273,7 +5541,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B55" s="12">
         <v>2006</v>
@@ -4283,7 +5551,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B56" s="12">
         <v>1</v>
@@ -4293,7 +5561,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B57" s="12">
         <v>1</v>
@@ -4303,7 +5571,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B58" s="12">
         <v>1</v>
@@ -4313,7 +5581,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B59" s="12">
         <v>2006</v>
@@ -4323,7 +5591,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B60" s="12">
         <v>12</v>
@@ -4333,7 +5601,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B61" s="12">
         <v>31</v>
@@ -4343,7 +5611,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B62" s="12">
         <v>24</v>
@@ -4359,48 +5627,48 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B65" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D65" s="14">
         <v>1.9528741509529837E-2</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B66" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D66" s="13">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -4411,37 +5679,37 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B69" s="14">
         <v>2.0648572594225215E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B70" s="13">
         <v>2E-8</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -4453,36 +5721,36 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B72" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D72" s="14">
         <v>1.1841887362491711E-2</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B73" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D73" s="14">
         <v>2.2590009128958689E-2</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4493,30 +5761,30 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B75" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D75" s="14">
         <v>6.2433901191501419E-2</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B76" s="14">
         <v>2.5158160216169324E-2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D76" s="14">
         <v>2.5158160216169324E-2</v>
@@ -4531,32 +5799,32 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="B78" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D78" s="12">
         <f>261*0.08/8760</f>
         <v>2.3835616438356165E-3</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B79" s="12">
         <v>0</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D79" s="12">
         <v>0</v>
@@ -4565,13 +5833,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="B80" s="12">
         <v>0</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D80" s="12">
         <v>0</v>
@@ -4580,7 +5848,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B81" s="12">
         <v>0.9</v>
@@ -4593,13 +5861,13 @@
     </row>
     <row r="82" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B82" s="12">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D82" s="12">
         <v>1.0000000000000001E-5</v>
@@ -4611,19 +5879,19 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B83" s="12">
         <v>6</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D83" s="12">
         <v>6</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -4634,70 +5902,70 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="B85" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D85" s="12">
         <f>0.3*0.08/8760</f>
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B86" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D86" s="12">
         <f>1100*0.08/8760</f>
         <v>1.0045662100456621E-2</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B87" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D87" s="12">
         <f>4600*0.08/8760</f>
         <v>4.2009132420091327E-2</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B88" s="12">
         <v>0</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D88" s="12">
         <v>0</v>
@@ -4706,13 +5974,13 @@
     </row>
     <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B89" s="12">
         <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D89" s="12">
         <v>0</v>
@@ -4721,7 +5989,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B90" s="12">
         <v>0.3</v>
@@ -4741,13 +6009,13 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B92" s="12">
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D92" s="12">
         <v>10</v>
@@ -4763,51 +6031,51 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C94" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C95" s="4"/>
     </row>
     <row r="96" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4815,7 +6083,7 @@
     </row>
     <row r="98" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B98" s="6">
         <v>0.5</v>
@@ -4850,7 +6118,7 @@
     </row>
     <row r="99" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B99" s="6">
         <v>-1</v>
@@ -4885,13 +6153,13 @@
     </row>
     <row r="101" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B101" s="11"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>